<commit_message>
Add data driven testing
</commit_message>
<xml_diff>
--- a/excelData/accountData.xlsx
+++ b/excelData/accountData.xlsx
@@ -7,10 +7,9 @@
     <workbookView windowWidth="23040" windowHeight="9420"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AccountData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <oleSize ref="A1:B8"/>
 </workbook>
 </file>
 
@@ -87,7 +86,22 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,14 +112,6 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -113,22 +119,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -150,30 +148,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -181,21 +165,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -217,6 +186,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -227,6 +226,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -255,55 +261,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -315,127 +429,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,36 +466,6 @@
       </top>
       <bottom style="medium">
         <color rgb="FFDEE2E6"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -518,11 +494,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -553,6 +535,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -561,159 +558,173 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="10" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="10" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -778,7 +789,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1038,108 +1049,108 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="19.4444444444444" customWidth="1"/>
+    <col min="1" max="1" width="25.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="19.7777777777778" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>123456789</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>5245</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" ht="15.15" spans="1:2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" ht="15" customHeight="1" spans="1:2">
-      <c r="A12" s="3" t="s">
+    <row r="12" ht="29.55" spans="1:2">
+      <c r="A12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>123</v>
       </c>
     </row>

</xml_diff>